<commit_message>
add difficulties and landscape tokens set
</commit_message>
<xml_diff>
--- a/game_design/game_config.xlsx
+++ b/game_design/game_config.xlsx
@@ -4618,7 +4618,7 @@
         <v>1.0</v>
       </c>
       <c r="D2" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -4635,7 +4635,7 @@
         <v>1.0</v>
       </c>
       <c r="D3" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>19</v>
@@ -4652,7 +4652,7 @@
         <v>2.0</v>
       </c>
       <c r="D4" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -4669,7 +4669,7 @@
         <v>2.0</v>
       </c>
       <c r="D5" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>18</v>
@@ -5274,7 +5274,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>51</v>

</xml_diff>